<commit_message>
- Implemented local database to store and retrieve event data - Implemented E-Mail downloader service to fetch emails from user's inbox - Implemented Event Recognizer service to extract event details from email content - Implemented Event Duplicator service to avoid duplicate event entries in the database - Implemented Event Pipeline service to orchestrate the email processing and event extraction workflow - Added Dropdown sorting button to EventList component
</commit_message>
<xml_diff>
--- a/project/backend/data/temp_emails/extracted_event_info.xlsx
+++ b/project/backend/data/temp_emails/extracted_event_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>Title</t>
   </si>
@@ -49,7 +49,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Walk&amp;Talk – gemeinsam spazieren, quatschen, Leute treffen</t>
+    <t>Walk&amp;Talk</t>
   </si>
   <si>
     <t>Eröffnung der Sonderausstellung „Kunst / Macht. Rubens’ Medici-Zyklus und der gedruckte Kanon“</t>
@@ -58,49 +58,52 @@
     <t>Sonderausstellung „Kunst / Macht. Rubens’ Medici-Zyklus und der gedruckte Kanon“</t>
   </si>
   <si>
-    <t>22.11.25</t>
-  </si>
-  <si>
-    <t>28.11.25</t>
-  </si>
-  <si>
-    <t>12.12.25</t>
-  </si>
-  <si>
-    <t>13.12.25</t>
-  </si>
-  <si>
-    <t>16.01.26</t>
-  </si>
-  <si>
-    <t>20. November 2025</t>
-  </si>
-  <si>
-    <t>21. November 2025</t>
-  </si>
-  <si>
-    <t>18. Januar 2026</t>
-  </si>
-  <si>
-    <t>15:00 Uhr</t>
-  </si>
-  <si>
-    <t>19 Uhr</t>
-  </si>
-  <si>
-    <t>10 Uhr</t>
-  </si>
-  <si>
-    <t>16:30 Uhr</t>
-  </si>
-  <si>
-    <t>Gemeinsam spazieren gehen, quatschen, neue Leute kennenlernen oder vertraulich mit studentischen Hosts reden (#mentalhealthmatters), wenn dir etwas auf dem Herzen liegt? Klingt gut? Dann komm vorbei zu Walk&amp;Talk – einem Angebot von und für Studierende!</t>
-  </si>
-  <si>
-    <t>Die Eröffnung der Sonderausstellung „Kunst / Macht. Rubens’ Medici-Zyklus und der gedruckte Kanon“ findet am Donnerstag, den 20. November 2025, um 19 Uhr in der Schlosskirche von Schloss Hohentübingen statt.</t>
-  </si>
-  <si>
-    <t>Die Ausstellung wurde von Ariane Koller und Anna Pawlak in Zusammenarbeit mit dem SFB 1391 Andere Ästhetik und dem Museum der Universität Tübingen MUT konzipiert. Sie wird von einer gleichnamigen Publikation begleitet. Vom 21. November 2025 bis 18. Januar 2026 zeigt die Graphische Sammlung des Kunsthistorischen Instituts auf Schloss Hohentübingen erstmals das druckgraphische Galeriewerk La Gallerie du Palais du Luxembourg (1710) mit 27 Kupferstichen nach dem Medici-Zyklus von Peter Paul Rubens. Die Ausstellung macht sichtbar, wie diese eindrucksvollen Druckgraphiken Rubens’ monumentale Bildfolge im frühen 18. Jahrhundert europaweit verbreiteten, neu interpretierten und kunsthistorisch prägend machten. Sie zeigt zugleich die Bedeutung des Galeriewerks als Vermittlungsmedium und als eigenständiges Kunstobjekt, das die Rezeption und Deutung des Zyklus über Jahrhunderte beeinflusste.</t>
+    <t>11/22/2025</t>
+  </si>
+  <si>
+    <t>11/28/2025</t>
+  </si>
+  <si>
+    <t>12/12/2025</t>
+  </si>
+  <si>
+    <t>12/13/2025</t>
+  </si>
+  <si>
+    <t>01/16/2026</t>
+  </si>
+  <si>
+    <t>11/20/2025</t>
+  </si>
+  <si>
+    <t>11/21/2025</t>
+  </si>
+  <si>
+    <t>01/18/2026</t>
+  </si>
+  <si>
+    <t>03:00 PM</t>
+  </si>
+  <si>
+    <t>07:00 PM</t>
+  </si>
+  <si>
+    <t>10:00 AM</t>
+  </si>
+  <si>
+    <t>04:30 PM</t>
+  </si>
+  <si>
+    <t>05:00 PM</t>
+  </si>
+  <si>
+    <t>Gemeinsam spazieren gehen, quatschen, neue Leute kennenlernen oder vertraulich mit studentischen Hosts über mentale Gesundheit reden. Ein Angebot von und für Studierende.</t>
+  </si>
+  <si>
+    <t>Die Eröffnung der Sonderausstellung „Kunst / Macht. Rubens’ Medici-Zyklus und der gedruckte Kanon“ findet in der Schlosskirche von Schloss Hohentübingen statt. Die Ausstellung wurde von Ariane Koller und Anna Pawlak in Zusammenarbeit mit dem SFB 1391 Andere Ästhetik und dem Museum der Universität Tübingen MUT konzipiert. Sie wird von einer gleichnamigen Publikation begleitet.</t>
+  </si>
+  <si>
+    <t>Vom 21. November 2025 bis 18. Januar 2026 zeigt die Graphische Sammlung des Kunsthistorischen Instituts auf Schloss Hohentübingen erstmals das druckgraphische Galeriewerk La Gallerie du Palais du Luxembourg (1710) mit 27 Kupferstichen nach dem Medici-Zyklus von Peter Paul Rubens. Die Ausstellung macht sichtbar, wie diese eindrucksvollen Druckgraphiken Rubens’ monumentale Bildfolge im frühen 18. Jahrhundert europaweit verbreiteten, neu interpretierten und kunsthistorisch prägend machten. Sie zeigt zugleich die Bedeutung des Galeriewerks als Vermittlungsmedium und als eigenständiges Kunstobjekt, das die Rezeption und Deutung des Zyklus über Jahrhunderte beeinflusste.</t>
   </si>
   <si>
     <t>Taubenhaus (auf der Neckarinsel)</t>
@@ -550,19 +553,19 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -582,19 +585,19 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -614,19 +617,19 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -646,19 +649,19 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -678,19 +681,19 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -707,16 +710,16 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -733,19 +736,22 @@
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>